<commit_message>
finished removing unnecesarry rows. working on put txpower same row as evm
</commit_message>
<xml_diff>
--- a/test-orig.xlsx
+++ b/test-orig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene\Documents\code\QSPRparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19485DED-D39F-413D-B119-DA5E8C45E486}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFF6948-E5BC-42AE-9CFD-15D189C72385}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{9F3919FB-ADB3-4E00-A4FF-6BC167CFA25D}"/>
   </bookViews>
@@ -573,19 +573,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D363B752-B9AE-4A87-82EB-02E1BD507AF8}">
   <dimension ref="A1:V1733"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="80.44140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.109375" bestFit="1" customWidth="1"/>

</xml_diff>